<commit_message>
update class_specifications and upload class UML
</commit_message>
<xml_diff>
--- a/sprint1/class_specifications.xlsx
+++ b/sprint1/class_specifications.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\umbc\spring23\cmsc447\project\CMSC_447_Group_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\umbc\spring23\cmsc447\project\sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045476F0-B635-4557-82C4-1CC041334D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06709D6B-7378-4EA5-BFBE-8ABD863A5E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-18260" yWindow="3260" windowWidth="17280" windowHeight="8900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirement" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t xml:space="preserve">Description </t>
   </si>
@@ -351,13 +351,6 @@
 decrease the score if the the player gets hit by a downgrade of minus point</t>
   </si>
   <si>
-    <t>-current_score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-+get/set score</t>
-  </si>
-  <si>
     <t>Gaming Flow</t>
   </si>
   <si>
@@ -394,6 +387,52 @@
 +get/set pos_x
 +get/set pos_y
 +hit(falling_object)</t>
+  </si>
+  <si>
+    <t>control_system</t>
+  </si>
+  <si>
+    <t>keep track of the game flow</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>connect with API stuffs: database, players,…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+-current_score
+-factor
+_end_game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
++get/set score
++get/set factor
++get end_game
+-set end_game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+-control_system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+-player
+-scoring_system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
++end_game
++get_scoring_system
++get_player</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
++get/set ranking_db
++get/set player
+</t>
   </si>
 </sst>
 </file>
@@ -470,7 +509,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -490,6 +529,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -28757,10 +28797,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1002"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.609375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -28808,12 +28848,12 @@
       <c r="Z1" s="6"/>
     </row>
     <row r="2" spans="1:26" ht="12.3" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -28845,10 +28885,10 @@
         <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -29061,10 +29101,10 @@
         <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -29089,13 +29129,19 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="7" t="s">
-        <v>42</v>
+    <row r="10" spans="1:26" s="7" customFormat="1" ht="49.2" x14ac:dyDescent="0.4">
+      <c r="A10" s="3" t="s">
+        <v>49</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -29119,15 +29165,19 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
-        <v>43</v>
+    <row r="11" spans="1:26" s="7" customFormat="1" ht="49.2" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
+        <v>51</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>44</v>
+      <c r="B11" s="3" t="s">
+        <v>52</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -29151,15 +29201,13 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
-        <v>45</v>
+    <row r="12" spans="1:26" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A12" s="8" t="s">
+        <v>40</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -29183,12 +29231,12 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" ht="24.6" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -29215,9 +29263,13 @@
       <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
+    <row r="14" spans="1:26" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -29244,8 +29296,12 @@
       <c r="Z14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -29607,7 +29663,7 @@
       <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
     </row>
-    <row r="28" spans="1:26" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -29635,7 +29691,7 @@
       <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
     </row>
-    <row r="29" spans="1:26" ht="12.3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -56907,10 +56963,66 @@
       <c r="Y1002" s="3"/>
       <c r="Z1002" s="3"/>
     </row>
+    <row r="1003" spans="1:26" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A1003" s="3"/>
+      <c r="B1003" s="3"/>
+      <c r="C1003" s="3"/>
+      <c r="D1003" s="3"/>
+      <c r="E1003" s="3"/>
+      <c r="F1003" s="3"/>
+      <c r="G1003" s="3"/>
+      <c r="H1003" s="3"/>
+      <c r="I1003" s="3"/>
+      <c r="J1003" s="3"/>
+      <c r="K1003" s="3"/>
+      <c r="L1003" s="3"/>
+      <c r="M1003" s="3"/>
+      <c r="N1003" s="3"/>
+      <c r="O1003" s="3"/>
+      <c r="P1003" s="3"/>
+      <c r="Q1003" s="3"/>
+      <c r="R1003" s="3"/>
+      <c r="S1003" s="3"/>
+      <c r="T1003" s="3"/>
+      <c r="U1003" s="3"/>
+      <c r="V1003" s="3"/>
+      <c r="W1003" s="3"/>
+      <c r="X1003" s="3"/>
+      <c r="Y1003" s="3"/>
+      <c r="Z1003" s="3"/>
+    </row>
+    <row r="1004" spans="1:26" ht="12.3" x14ac:dyDescent="0.4">
+      <c r="A1004" s="3"/>
+      <c r="B1004" s="3"/>
+      <c r="C1004" s="3"/>
+      <c r="D1004" s="3"/>
+      <c r="E1004" s="3"/>
+      <c r="F1004" s="3"/>
+      <c r="G1004" s="3"/>
+      <c r="H1004" s="3"/>
+      <c r="I1004" s="3"/>
+      <c r="J1004" s="3"/>
+      <c r="K1004" s="3"/>
+      <c r="L1004" s="3"/>
+      <c r="M1004" s="3"/>
+      <c r="N1004" s="3"/>
+      <c r="O1004" s="3"/>
+      <c r="P1004" s="3"/>
+      <c r="Q1004" s="3"/>
+      <c r="R1004" s="3"/>
+      <c r="S1004" s="3"/>
+      <c r="T1004" s="3"/>
+      <c r="U1004" s="3"/>
+      <c r="V1004" s="3"/>
+      <c r="W1004" s="3"/>
+      <c r="X1004" s="3"/>
+      <c r="Y1004" s="3"/>
+      <c r="Z1004" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A12:D12"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:Z1">
     <cfRule type="colorScale" priority="1">

</xml_diff>